<commit_message>
feat [#Tutorial 15] : Add plot data table from excel
</commit_message>
<xml_diff>
--- a/sample data.xlsx
+++ b/sample data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Giga\Dokumen\Cinovasi\Project\Demo\PSAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C8AC0A2-6608-4BEE-BFB2-F96BB77D99E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6594F88-A544-4FFE-9111-920B58C0B3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{7D387DD7-3485-4AE8-B7CF-F892E3A33F8D}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +412,8 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <f>A2*2</f>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +421,8 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <f t="shared" ref="B3:B21" si="0">A3*2</f>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -428,7 +430,8 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,6 +439,7 @@
         <v>4</v>
       </c>
       <c r="B5">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -444,7 +448,8 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +457,8 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,7 +466,8 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>64</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,7 +475,8 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>128</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,7 +484,8 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>256</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +493,8 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>512</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -492,7 +502,8 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1024</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -500,7 +511,8 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2048</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +520,8 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4096</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,8 +529,8 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <f>B14*2</f>
-        <v>8192</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -525,8 +538,8 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:B21" si="0">B15*2</f>
-        <v>16384</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -535,7 +548,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>32768</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -544,7 +557,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>65536</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,7 +566,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>131072</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -562,7 +575,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>262144</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -571,7 +584,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>524288</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat [#Tutorial 17] : Add row data table from UI
</commit_message>
<xml_diff>
--- a/sample data.xlsx
+++ b/sample data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Giga\Dokumen\Cinovasi\Project\Demo\PSAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6594F88-A544-4FFE-9111-920B58C0B3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6E2828-1E29-48E8-B643-20BAA9774428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{7D387DD7-3485-4AE8-B7CF-F892E3A33F8D}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{7D387DD7-3485-4AE8-B7CF-F892E3A33F8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,12 +35,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Mane</t>
+  </si>
+  <si>
+    <t>Virgil</t>
+  </si>
+  <si>
+    <t>Firmino</t>
+  </si>
+  <si>
+    <t>Salah</t>
   </si>
 </sst>
 </file>
@@ -393,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702AB608-B2CA-4FFF-BF3B-908E4659A164}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -590,4 +609,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB0CA90-6108-42E6-B8E5-8946C9E51AE7}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>